<commit_message>
first beta release 3.0.0
</commit_message>
<xml_diff>
--- a/application/views/rpt/xlsx/TPL_EventList.xlsx
+++ b/application/views/rpt/xlsx/TPL_EventList.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505"/>
@@ -12,30 +12,21 @@
     <sheet name="Лист3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Лист1!$A$1:$G$7</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Лист1!$A$1:$F$4</definedName>
   </definedNames>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>п/п</t>
   </si>
   <si>
-    <t>Телефон</t>
-  </si>
-  <si>
     <t>Доп-но</t>
   </si>
   <si>
-    <t>Название</t>
-  </si>
-  <si>
-    <t>Адрес</t>
-  </si>
-  <si>
     <t>{$v[items][loop][i]}</t>
   </si>
   <si>
@@ -57,19 +48,16 @@
     <t>Список "{$v[label]}" от {$v[date]}</t>
   </si>
   <si>
-    <t>Получатель (Клиент)</t>
-  </si>
-  <si>
-    <t>Автомобиль:</t>
-  </si>
-  <si>
-    <t>Начальный пробег:</t>
-  </si>
-  <si>
-    <t>Конечный пробег:</t>
-  </si>
-  <si>
-    <t>Оплата</t>
+    <t>Задание</t>
+  </si>
+  <si>
+    <t>Получатель</t>
+  </si>
+  <si>
+    <t>Место</t>
+  </si>
+  <si>
+    <t>Контакт</t>
   </si>
 </sst>
 </file>
@@ -137,7 +125,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -153,26 +141,6 @@
         <color indexed="64"/>
       </right>
       <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -197,7 +165,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -207,6 +175,18 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -215,31 +195,6 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -542,10 +497,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:H10"/>
+  <dimension ref="B1:G7"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -556,126 +511,90 @@
     <col min="4" max="4" width="25.7109375" style="1" customWidth="1"/>
     <col min="5" max="5" width="23.85546875" style="1" customWidth="1"/>
     <col min="6" max="6" width="12.140625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="10.5703125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="15.140625" style="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="1"/>
+    <col min="7" max="7" width="15.140625" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B1" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
+    <row r="1" spans="2:7" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B1" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
     </row>
-    <row r="2" spans="2:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="C2" s="8"/>
-      <c r="D2" s="9"/>
+    <row r="2" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
     </row>
-    <row r="3" spans="2:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="C3" s="8"/>
-      <c r="D3" s="10"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
+    <row r="3" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>1</v>
+      </c>
     </row>
-    <row r="4" spans="2:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4" s="8"/>
-      <c r="D4" s="10"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
+    <row r="4" spans="2:7" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
     </row>
-    <row r="6" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="C6" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="D6" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="E6" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="F6" s="13" t="s">
-        <v>1</v>
-      </c>
-      <c r="G6" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="H6" s="13" t="s">
-        <v>2</v>
-      </c>
+    <row r="6" spans="2:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C6" s="9"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="9"/>
     </row>
-    <row r="7" spans="2:8" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="D7" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="E7" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="F7" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="G7" s="11"/>
-      <c r="H7" s="15" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-    </row>
-    <row r="9" spans="2:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
-    </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="6"/>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C7" s="10"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="10"/>
+      <c r="F7" s="10"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
-    <mergeCell ref="C9:F9"/>
-    <mergeCell ref="C10:F10"/>
-    <mergeCell ref="B1:G1"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B3:C3"/>
+  <mergeCells count="3">
+    <mergeCell ref="C6:F6"/>
+    <mergeCell ref="C7:F7"/>
+    <mergeCell ref="B1:F1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>

</xml_diff>